<commit_message>
Doc stats March 2020
</commit_message>
<xml_diff>
--- a/docs/GitHubIssues.xlsx
+++ b/docs/GitHubIssues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwren\Git\bwren\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE52B2A3-40F3-424E-A0FD-C7591E4E589A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BE860F-57CC-493E-9C48-D2514F41140F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="735" windowWidth="47985" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="795" yWindow="585" windowWidth="39960" windowHeight="16845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GitHubIssues" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3834" uniqueCount="2331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4074" uniqueCount="2483">
   <si>
     <t>shashishailaj</t>
   </si>
@@ -7026,6 +7026,462 @@
   </si>
   <si>
     <t>Article</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/51360</t>
+  </si>
+  <si>
+    <t>Listing Windows 10 Enterprise multi-session</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/51336</t>
+  </si>
+  <si>
+    <t>OMS agent omsconfig not picking the portal configuration automatically after installation</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/agent-linux-troubleshoot.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/agent-linux-troubleshoot.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/51171</t>
+  </si>
+  <si>
+    <t>Template deployment fails with errror "Bad request, Please check the CustomerId, Path and Key for restricted symbols"</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/51109</t>
+  </si>
+  <si>
+    <t>azure log analytics query power bi</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/powerbi.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/powerbi.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/51014</t>
+  </si>
+  <si>
+    <t>Disabling full SQL Query in ASP.Net Core</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/asp-net-dependencies.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/asp-net-dependencies.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50996</t>
+  </si>
+  <si>
+    <t>Action Type needs to be updated</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/action-groups.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/action-groups.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50884</t>
+  </si>
+  <si>
+    <t>Disable getting alerted when a metric alert is marked as resolved by Azure?</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50880</t>
+  </si>
+  <si>
+    <t>Alternatives include this very solution</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50837</t>
+  </si>
+  <si>
+    <t>Update Circonus logo on Azure Partners page</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/partners.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/partners.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50782</t>
+  </si>
+  <si>
+    <t>Application Insights Continuous Export reliability</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/export-telemetry.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/export-telemetry.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50718</t>
+  </si>
+  <si>
+    <t>"Upgrade all clusters using Bash in Azure Command Shell" NOT WORKING</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/insights/container-insights-update-metrics.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/insights/container-insights-update-metrics.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorrect "PrivateConfig" Json example </t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/diagnostics-extension-schema-windows.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/diagnostics-extension-schema-windows.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50700</t>
+  </si>
+  <si>
+    <t>No description of the access control types</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/manage-access.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/manage-access.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50699</t>
+  </si>
+  <si>
+    <t>Trying to set up a Secure WebHook integration with Monitoring Alerts but this document and others are sparse on the topic of Secure Webhook</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50698</t>
+  </si>
+  <si>
+    <t>Note box incorrect?</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50687</t>
+  </si>
+  <si>
+    <t>Make a distinction between App Service OS for agent-based app monitoring</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50619</t>
+  </si>
+  <si>
+    <t>Re-write this entire page.</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/asp-net-trace-logs.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/asp-net-trace-logs.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50612</t>
+  </si>
+  <si>
+    <t>Not able to change colors of chart lines</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/metrics-charts.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/metrics-charts.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50602</t>
+  </si>
+  <si>
+    <t>Document the list of common unsupported technology</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50505</t>
+  </si>
+  <si>
+    <t>Is there a way to edit or delete saved functions?</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/log-query/functions.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/log-query/functions.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50502</t>
+  </si>
+  <si>
+    <t>Set-OMSGatewayRelayProxy "Password" parameter seems to require SecureString value</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/gateway.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/gateway.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50394</t>
+  </si>
+  <si>
+    <t>Is there a reason why Open Debug Snapshot is not showing</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/snapshot-debugger.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/snapshot-debugger.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50377</t>
+  </si>
+  <si>
+    <t>Is it possible to configure ApplicationInsights 's AvailabilityTests for an end point (of AppService) hosted in ASE?</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50363</t>
+  </si>
+  <si>
+    <t>Document all available ApplicationInsightsServiceOptions</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50262</t>
+  </si>
+  <si>
+    <t>.Net Framework only 4.5, 4.6 supported - not higher</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50209</t>
+  </si>
+  <si>
+    <t>APPINSIGHTS_INSTRUMENTATIONKEY and APPLICATIONINSIGHTS_CONNECTION_STRING</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50206</t>
+  </si>
+  <si>
+    <t>Azure Monitor for VMs is not in preview anymore.</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50121</t>
+  </si>
+  <si>
+    <t>Next Steps: "Create metric alerts using ARM Templates" link out of date</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can we make it clear for different data types ? </t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/workbooks-text.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/workbooks-text.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50027</t>
+  </si>
+  <si>
+    <t>Hard delete does not work</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50015</t>
+  </si>
+  <si>
+    <t>Availability test template add parameter for 'Content Match' success criteria</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/50006</t>
+  </si>
+  <si>
+    <t>Please document if there are any limits and restrictions to the number of continuous jobs.</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49998</t>
+  </si>
+  <si>
+    <t>Missing docs for Microsoft.Web</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49965</t>
+  </si>
+  <si>
+    <t>RHEL 8 Support</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/insights/vminsights-enable-overview.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/insights/vminsights-enable-overview.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49951</t>
+  </si>
+  <si>
+    <t>Typo ""</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49944</t>
+  </si>
+  <si>
+    <t># Custom Logs script part</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49939</t>
+  </si>
+  <si>
+    <t>-countername in code part # Windows Event</t>
+  </si>
+  <si>
+    <t>AjayKumar-MSFT</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49930</t>
+  </si>
+  <si>
+    <t>In case of Multi Container in App Service how can we monitor each of the Containers</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/docker.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/docker.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49911</t>
+  </si>
+  <si>
+    <t>Example ARM template workspace API is not documented in the official ARM template references</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49908</t>
+  </si>
+  <si>
+    <t>Boot diagnostics element missing</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49837</t>
+  </si>
+  <si>
+    <t>Is there a way to get AzureMetrics information using a REST Api?</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/insights/azure-sql.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/insights/azure-sql.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49818</t>
+  </si>
+  <si>
+    <t>To detect changes in dependencies, Change Analysis checks the web app's DNS record</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49688</t>
+  </si>
+  <si>
+    <t>Should be marked as Deprecated or Obsolete - can no longer create "Classic" alerts, and they will stop working in June 2020.</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/alerts-enable-template.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/alerts-enable-template.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49639</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Data Types dont match inside the Storage blob location </t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49605</t>
+  </si>
+  <si>
+    <t>Cross-App Insights Resource Application Map</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49589</t>
+  </si>
+  <si>
+    <t>How to configure QUEUE PROPERTIES Diagnostics settings for Azure Storage Account using ARM</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49575</t>
+  </si>
+  <si>
+    <t>Resource column also gone</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/diagnostic-settings-legacy.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/diagnostic-settings-legacy.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49574</t>
+  </si>
+  <si>
+    <t>Failure enabling Azure Monitor for Containers</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/insights/container-insights-overview.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/insights/container-insights-overview.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49551</t>
+  </si>
+  <si>
+    <t>Debian 10 Buster</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49496</t>
+  </si>
+  <si>
+    <t>Azure Data Lake gen 2 compatibility</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49466</t>
+  </si>
+  <si>
+    <t>Automate custom reports with Azure Application Insights data</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/automate-custom-reports.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/automate-custom-reports.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49433</t>
+  </si>
+  <si>
+    <t>Clearly document the service tag</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49369</t>
+  </si>
+  <si>
+    <t>REST API Monitor registered provider not found</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/insights/vminsights-health.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/insights/vminsights-health.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49358</t>
+  </si>
+  <si>
+    <t>Log Analytics Authentication</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete or Rewrite this article </t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/opencensus-go.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/opencensus-go.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49335</t>
+  </si>
+  <si>
+    <t>Delete this article</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/app/opencensus-local-forwarder.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/app/opencensus-local-forwarder.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49299</t>
+  </si>
+  <si>
+    <t>How to query activity logs in a Storage account?</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/platform/resource-logs-collect-storage.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/platform/resource-logs-collect-storage.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49275</t>
+  </si>
+  <si>
+    <t>Existing savedsearches return 409 when deployed again</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/insights/solutions-resources-searches-alerts.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/insights/solutions-resources-searches-alerts.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49263</t>
+  </si>
+  <si>
+    <t>is that a typo?</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/insights/sql-assessment.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/insights/sql-assessment.md)</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49252</t>
+  </si>
+  <si>
+    <t>Microsoft.Web/sites (excluding functions) : CpuTime is not available when selecting function app</t>
+  </si>
+  <si>
+    <t>https://github.com/MicrosoftDocs/azure-docs/issues/49237</t>
+  </si>
+  <si>
+    <t>Non-existent pricing tier</t>
+  </si>
+  <si>
+    <t>[articles/azure-monitor/learn/tutorial-resource-logs.md](https://github.com/Microsoft/azure-docs/blob/master/articles/azure-monitor/learn/tutorial-resource-logs.md)</t>
   </si>
 </sst>
 </file>
@@ -7869,9 +8325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3087"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12111,7 +12565,7 @@
         <v>2122</v>
       </c>
       <c r="F202" t="str">
-        <f t="shared" ref="F202:F265" si="4">"http://docs.microsoft.com/azure/azure-monitor" &amp; SUBSTITUTE(SUBSTITUTE(LEFT(E202,FIND("]",E202)-1),"[articles",""),".md","")</f>
+        <f t="shared" ref="F202:F264" si="4">"http://docs.microsoft.com/azure/azure-monitor" &amp; SUBSTITUTE(SUBSTITUTE(LEFT(E202,FIND("]",E202)-1),"[articles",""),".md","")</f>
         <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/alerts-log</v>
       </c>
     </row>
@@ -18773,7 +19227,7 @@
         <v>2170</v>
       </c>
       <c r="F523" t="str">
-        <f t="shared" ref="F522:F585" si="9">"http://docs.microsoft.com/azure/azure-monitor" &amp; SUBSTITUTE(SUBSTITUTE(LEFT(E523,FIND("]",E523)-1),"[articles",""),".md","")</f>
+        <f t="shared" ref="F523:F585" si="9">"http://docs.microsoft.com/azure/azure-monitor" &amp; SUBSTITUTE(SUBSTITUTE(LEFT(E523,FIND("]",E523)-1),"[articles",""),".md","")</f>
         <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/alerts-unified-log</v>
       </c>
     </row>
@@ -26687,7 +27141,7 @@
         <v>2150</v>
       </c>
       <c r="F906" t="str">
-        <f t="shared" ref="F906:F966" si="15">"http://docs.microsoft.com/azure/azure-monitor" &amp; SUBSTITUTE(SUBSTITUTE(LEFT(E906,FIND("]",E906)-1),"[articles",""),".md","")</f>
+        <f t="shared" ref="F906:F969" si="15">"http://docs.microsoft.com/azure/azure-monitor" &amp; SUBSTITUTE(SUBSTITUTE(LEFT(E906,FIND("]",E906)-1),"[articles",""),".md","")</f>
         <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/alerts-activity-log</v>
       </c>
     </row>
@@ -27938,225 +28392,1323 @@
       </c>
     </row>
     <row r="967" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A967" s="1"/>
+      <c r="A967" s="1">
+        <v>43921.614965277775</v>
+      </c>
+      <c r="B967" t="s">
+        <v>31</v>
+      </c>
+      <c r="C967" t="s">
+        <v>2331</v>
+      </c>
+      <c r="D967" t="s">
+        <v>2332</v>
+      </c>
+      <c r="E967" t="s">
+        <v>106</v>
+      </c>
+      <c r="F967" t="str">
+        <f t="shared" si="15"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/log-analytics-agent</v>
+      </c>
     </row>
     <row r="968" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A968" s="1"/>
+      <c r="A968" s="1">
+        <v>43921.361435185187</v>
+      </c>
+      <c r="B968" t="s">
+        <v>10</v>
+      </c>
+      <c r="C968" t="s">
+        <v>2333</v>
+      </c>
+      <c r="D968" t="s">
+        <v>2334</v>
+      </c>
+      <c r="E968" t="s">
+        <v>2335</v>
+      </c>
+      <c r="F968" t="str">
+        <f t="shared" si="15"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/agent-linux-troubleshoot</v>
+      </c>
     </row>
     <row r="969" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A969" s="1"/>
+      <c r="A969" s="1">
+        <v>43919.513055555559</v>
+      </c>
+      <c r="B969" t="s">
+        <v>10</v>
+      </c>
+      <c r="C969" t="s">
+        <v>2336</v>
+      </c>
+      <c r="D969" t="s">
+        <v>2337</v>
+      </c>
+      <c r="E969" t="s">
+        <v>145</v>
+      </c>
+      <c r="F969" t="str">
+        <f t="shared" si="15"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/template-workspace-configuration</v>
+      </c>
     </row>
     <row r="970" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A970" s="1"/>
+      <c r="A970" s="1">
+        <v>43917.66333333333</v>
+      </c>
+      <c r="B970" t="s">
+        <v>54</v>
+      </c>
+      <c r="C970" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D970" t="s">
+        <v>2339</v>
+      </c>
+      <c r="E970" t="s">
+        <v>2340</v>
+      </c>
+      <c r="F970" t="str">
+        <f t="shared" ref="F970:F1027" si="16">"http://docs.microsoft.com/azure/azure-monitor" &amp; SUBSTITUTE(SUBSTITUTE(LEFT(E970,FIND("]",E970)-1),"[articles",""),".md","")</f>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/powerbi</v>
+      </c>
     </row>
     <row r="971" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A971" s="1"/>
+      <c r="A971" s="1">
+        <v>43916.633344907408</v>
+      </c>
+      <c r="B971" t="s">
+        <v>44</v>
+      </c>
+      <c r="C971" t="s">
+        <v>2341</v>
+      </c>
+      <c r="D971" t="s">
+        <v>2342</v>
+      </c>
+      <c r="E971" t="s">
+        <v>2343</v>
+      </c>
+      <c r="F971" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/asp-net-dependencies</v>
+      </c>
     </row>
     <row r="972" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A972" s="1"/>
+      <c r="A972" s="1">
+        <v>43916.463229166664</v>
+      </c>
+      <c r="B972" t="s">
+        <v>54</v>
+      </c>
+      <c r="C972" t="s">
+        <v>2344</v>
+      </c>
+      <c r="D972" t="s">
+        <v>2345</v>
+      </c>
+      <c r="E972" t="s">
+        <v>2346</v>
+      </c>
+      <c r="F972" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/action-groups</v>
+      </c>
     </row>
     <row r="973" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A973" s="1"/>
+      <c r="A973" s="1">
+        <v>43915.603252314817</v>
+      </c>
+      <c r="B973" t="s">
+        <v>54</v>
+      </c>
+      <c r="C973" t="s">
+        <v>2347</v>
+      </c>
+      <c r="D973" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E973" t="s">
+        <v>344</v>
+      </c>
+      <c r="F973" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/alerts-metric</v>
+      </c>
     </row>
     <row r="974" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A974" s="1"/>
+      <c r="A974" s="1">
+        <v>43915.568680555552</v>
+      </c>
+      <c r="B974" t="s">
+        <v>31</v>
+      </c>
+      <c r="C974" t="s">
+        <v>2349</v>
+      </c>
+      <c r="D974" t="s">
+        <v>2350</v>
+      </c>
+      <c r="E974" t="s">
+        <v>238</v>
+      </c>
+      <c r="F974" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/data-collector-api</v>
+      </c>
     </row>
     <row r="975" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A975" s="1"/>
+      <c r="A975" s="1">
+        <v>43914.972708333335</v>
+      </c>
+      <c r="B975" t="s">
+        <v>1</v>
+      </c>
+      <c r="C975" t="s">
+        <v>2351</v>
+      </c>
+      <c r="D975" t="s">
+        <v>2352</v>
+      </c>
+      <c r="E975" t="s">
+        <v>2353</v>
+      </c>
+      <c r="F975" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/partners</v>
+      </c>
     </row>
     <row r="976" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A976" s="1"/>
-    </row>
-    <row r="977" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A977" s="1"/>
-    </row>
-    <row r="978" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A978" s="1"/>
-    </row>
-    <row r="979" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A979" s="1"/>
-    </row>
-    <row r="980" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A980" s="1"/>
-    </row>
-    <row r="981" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A981" s="1"/>
-    </row>
-    <row r="982" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A982" s="1"/>
-    </row>
-    <row r="983" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A983" s="1"/>
-    </row>
-    <row r="984" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A984" s="1"/>
-    </row>
-    <row r="985" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A985" s="1"/>
-    </row>
-    <row r="986" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A986" s="1"/>
-    </row>
-    <row r="987" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A987" s="1"/>
-    </row>
-    <row r="988" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A988" s="1"/>
-    </row>
-    <row r="989" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A989" s="1"/>
-    </row>
-    <row r="990" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A990" s="1"/>
-    </row>
-    <row r="991" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A991" s="1"/>
-    </row>
-    <row r="992" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A992" s="1"/>
-    </row>
-    <row r="993" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A993" s="1"/>
-    </row>
-    <row r="994" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A994" s="1"/>
-    </row>
-    <row r="995" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A995" s="1"/>
-    </row>
-    <row r="996" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A996" s="1"/>
-    </row>
-    <row r="997" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A997" s="1"/>
-    </row>
-    <row r="998" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A998" s="1"/>
-    </row>
-    <row r="999" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A999" s="1"/>
-    </row>
-    <row r="1000" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1000" s="1"/>
-    </row>
-    <row r="1001" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1001" s="1"/>
-    </row>
-    <row r="1002" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1002" s="1"/>
-    </row>
-    <row r="1003" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1003" s="1"/>
-    </row>
-    <row r="1004" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1004" s="1"/>
-    </row>
-    <row r="1005" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1005" s="1"/>
-    </row>
-    <row r="1006" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1006" s="1"/>
-    </row>
-    <row r="1007" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1007" s="1"/>
-    </row>
-    <row r="1008" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1008" s="1"/>
-    </row>
-    <row r="1009" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1009" s="1"/>
-    </row>
-    <row r="1010" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1010" s="1"/>
-    </row>
-    <row r="1011" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1011" s="1"/>
-    </row>
-    <row r="1012" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1012" s="1"/>
-    </row>
-    <row r="1013" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1013" s="1"/>
-    </row>
-    <row r="1014" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1014" s="1"/>
-    </row>
-    <row r="1015" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1015" s="1"/>
-    </row>
-    <row r="1016" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1016" s="1"/>
-    </row>
-    <row r="1017" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1017" s="1"/>
-    </row>
-    <row r="1018" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1018" s="1"/>
-    </row>
-    <row r="1019" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1019" s="1"/>
-    </row>
-    <row r="1020" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1020" s="1"/>
-    </row>
-    <row r="1021" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1021" s="1"/>
-    </row>
-    <row r="1022" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1022" s="1"/>
-    </row>
-    <row r="1023" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1023" s="1"/>
-    </row>
-    <row r="1024" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1024" s="1"/>
-    </row>
-    <row r="1025" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1025" s="1"/>
-    </row>
-    <row r="1026" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1026" s="1"/>
-    </row>
-    <row r="1027" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1027" s="1"/>
-    </row>
-    <row r="1028" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A976" s="1">
+        <v>43914.469421296293</v>
+      </c>
+      <c r="B976" t="s">
+        <v>44</v>
+      </c>
+      <c r="C976" t="s">
+        <v>2354</v>
+      </c>
+      <c r="D976" t="s">
+        <v>2355</v>
+      </c>
+      <c r="E976" t="s">
+        <v>2356</v>
+      </c>
+      <c r="F976" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/export-telemetry</v>
+      </c>
+    </row>
+    <row r="977" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A977" s="1">
+        <v>43913.705370370371</v>
+      </c>
+      <c r="B977" t="s">
+        <v>54</v>
+      </c>
+      <c r="C977" t="s">
+        <v>2357</v>
+      </c>
+      <c r="D977" t="s">
+        <v>2358</v>
+      </c>
+      <c r="E977" t="s">
+        <v>2359</v>
+      </c>
+      <c r="F977" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/container-insights-update-metrics</v>
+      </c>
+    </row>
+    <row r="978" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A978" s="1">
+        <v>43913.554571759261</v>
+      </c>
+      <c r="B978" t="s">
+        <v>31</v>
+      </c>
+      <c r="C978" t="s">
+        <v>2360</v>
+      </c>
+      <c r="D978" t="s">
+        <v>2361</v>
+      </c>
+      <c r="E978" t="s">
+        <v>2362</v>
+      </c>
+      <c r="F978" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/diagnostics-extension-schema-windows</v>
+      </c>
+    </row>
+    <row r="979" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A979" s="1">
+        <v>43913.542002314818</v>
+      </c>
+      <c r="B979" t="s">
+        <v>10</v>
+      </c>
+      <c r="C979" t="s">
+        <v>2363</v>
+      </c>
+      <c r="D979" t="s">
+        <v>2364</v>
+      </c>
+      <c r="E979" t="s">
+        <v>2365</v>
+      </c>
+      <c r="F979" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/manage-access</v>
+      </c>
+    </row>
+    <row r="980" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A980" s="1">
+        <v>43913.540983796294</v>
+      </c>
+      <c r="B980" t="s">
+        <v>161</v>
+      </c>
+      <c r="C980" t="s">
+        <v>2366</v>
+      </c>
+      <c r="D980" t="s">
+        <v>2367</v>
+      </c>
+      <c r="E980" t="s">
+        <v>2346</v>
+      </c>
+      <c r="F980" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/action-groups</v>
+      </c>
+    </row>
+    <row r="981" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A981" s="1">
+        <v>43913.540335648147</v>
+      </c>
+      <c r="B981" t="s">
+        <v>10</v>
+      </c>
+      <c r="C981" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D981" t="s">
+        <v>2369</v>
+      </c>
+      <c r="E981" t="s">
+        <v>2365</v>
+      </c>
+      <c r="F981" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/manage-access</v>
+      </c>
+    </row>
+    <row r="982" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A982" s="1">
+        <v>43913.359965277778</v>
+      </c>
+      <c r="B982" t="s">
+        <v>35</v>
+      </c>
+      <c r="C982" t="s">
+        <v>2370</v>
+      </c>
+      <c r="D982" t="s">
+        <v>2371</v>
+      </c>
+      <c r="E982" t="s">
+        <v>80</v>
+      </c>
+      <c r="F982" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/azure-web-apps</v>
+      </c>
+    </row>
+    <row r="983" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A983" s="1">
+        <v>43911.052025462966</v>
+      </c>
+      <c r="B983" t="s">
+        <v>201</v>
+      </c>
+      <c r="C983" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D983" t="s">
+        <v>2373</v>
+      </c>
+      <c r="E983" t="s">
+        <v>2374</v>
+      </c>
+      <c r="F983" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/asp-net-trace-logs</v>
+      </c>
+    </row>
+    <row r="984" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A984" s="1">
+        <v>43910.8984375</v>
+      </c>
+      <c r="B984" t="s">
+        <v>11</v>
+      </c>
+      <c r="C984" t="s">
+        <v>2375</v>
+      </c>
+      <c r="D984" t="s">
+        <v>2376</v>
+      </c>
+      <c r="E984" t="s">
+        <v>2377</v>
+      </c>
+      <c r="F984" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/metrics-charts</v>
+      </c>
+    </row>
+    <row r="985" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A985" s="1">
+        <v>43910.828576388885</v>
+      </c>
+      <c r="B985" t="s">
+        <v>201</v>
+      </c>
+      <c r="C985" t="s">
+        <v>2378</v>
+      </c>
+      <c r="D985" t="s">
+        <v>2379</v>
+      </c>
+      <c r="E985" t="s">
+        <v>80</v>
+      </c>
+      <c r="F985" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/azure-web-apps</v>
+      </c>
+    </row>
+    <row r="986" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A986" s="1">
+        <v>43909.686724537038</v>
+      </c>
+      <c r="B986" t="s">
+        <v>54</v>
+      </c>
+      <c r="C986" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D986" t="s">
+        <v>2381</v>
+      </c>
+      <c r="E986" t="s">
+        <v>2382</v>
+      </c>
+      <c r="F986" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/log-query/functions</v>
+      </c>
+    </row>
+    <row r="987" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A987" s="1">
+        <v>43909.660671296297</v>
+      </c>
+      <c r="B987" t="s">
+        <v>54</v>
+      </c>
+      <c r="C987" t="s">
+        <v>2383</v>
+      </c>
+      <c r="D987" t="s">
+        <v>2384</v>
+      </c>
+      <c r="E987" t="s">
+        <v>2385</v>
+      </c>
+      <c r="F987" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/gateway</v>
+      </c>
+    </row>
+    <row r="988" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A988" s="1">
+        <v>43908.526400462964</v>
+      </c>
+      <c r="B988" t="s">
+        <v>47</v>
+      </c>
+      <c r="C988" t="s">
+        <v>2386</v>
+      </c>
+      <c r="D988" t="s">
+        <v>2387</v>
+      </c>
+      <c r="E988" t="s">
+        <v>2388</v>
+      </c>
+      <c r="F988" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/snapshot-debugger</v>
+      </c>
+    </row>
+    <row r="989" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A989" s="1">
+        <v>43908.228055555555</v>
+      </c>
+      <c r="B989" t="s">
+        <v>12</v>
+      </c>
+      <c r="C989" t="s">
+        <v>2389</v>
+      </c>
+      <c r="D989" t="s">
+        <v>2390</v>
+      </c>
+      <c r="E989" t="s">
+        <v>270</v>
+      </c>
+      <c r="F989" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/monitor-web-app-availability</v>
+      </c>
+    </row>
+    <row r="990" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A990" s="1">
+        <v>43907.939502314817</v>
+      </c>
+      <c r="B990" t="s">
+        <v>201</v>
+      </c>
+      <c r="C990" t="s">
+        <v>2391</v>
+      </c>
+      <c r="D990" t="s">
+        <v>2392</v>
+      </c>
+      <c r="E990" t="s">
+        <v>57</v>
+      </c>
+      <c r="F990" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/asp-net-core</v>
+      </c>
+    </row>
+    <row r="991" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A991" s="1">
+        <v>43906.744143518517</v>
+      </c>
+      <c r="B991" t="s">
+        <v>201</v>
+      </c>
+      <c r="C991" t="s">
+        <v>2393</v>
+      </c>
+      <c r="D991" t="s">
+        <v>2394</v>
+      </c>
+      <c r="E991" t="s">
+        <v>29</v>
+      </c>
+      <c r="F991" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/console</v>
+      </c>
+    </row>
+    <row r="992" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A992" s="1">
+        <v>43905.426134259258</v>
+      </c>
+      <c r="B992" t="s">
+        <v>201</v>
+      </c>
+      <c r="C992" t="s">
+        <v>2395</v>
+      </c>
+      <c r="D992" t="s">
+        <v>2396</v>
+      </c>
+      <c r="E992" t="s">
+        <v>80</v>
+      </c>
+      <c r="F992" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/azure-web-apps</v>
+      </c>
+    </row>
+    <row r="993" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A993" s="1">
+        <v>43905.242523148147</v>
+      </c>
+      <c r="B993" t="s">
+        <v>31</v>
+      </c>
+      <c r="C993" t="s">
+        <v>2397</v>
+      </c>
+      <c r="D993" t="s">
+        <v>2398</v>
+      </c>
+      <c r="E993" t="s">
+        <v>18</v>
+      </c>
+      <c r="F993" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/vminsights-overview</v>
+      </c>
+    </row>
+    <row r="994" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A994" s="1">
+        <v>43903.477835648147</v>
+      </c>
+      <c r="B994" t="s">
+        <v>341</v>
+      </c>
+      <c r="C994" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D994" t="s">
+        <v>2400</v>
+      </c>
+      <c r="E994" t="s">
+        <v>344</v>
+      </c>
+      <c r="F994" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/alerts-metric</v>
+      </c>
+    </row>
+    <row r="995" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A995" s="1">
+        <v>43902.99355324074</v>
+      </c>
+      <c r="B995" t="s">
+        <v>35</v>
+      </c>
+      <c r="C995" t="s">
+        <v>2401</v>
+      </c>
+      <c r="D995" t="s">
+        <v>2402</v>
+      </c>
+      <c r="E995" t="s">
+        <v>2403</v>
+      </c>
+      <c r="F995" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/workbooks-text</v>
+      </c>
+    </row>
+    <row r="996" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A996" s="1">
+        <v>43902.392650462964</v>
+      </c>
+      <c r="B996" t="s">
+        <v>54</v>
+      </c>
+      <c r="C996" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D996" t="s">
+        <v>2405</v>
+      </c>
+      <c r="E996" t="s">
+        <v>205</v>
+      </c>
+      <c r="F996" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/delete-workspace</v>
+      </c>
+    </row>
+    <row r="997" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A997" s="1">
+        <v>43902.247534722221</v>
+      </c>
+      <c r="B997" t="s">
+        <v>9</v>
+      </c>
+      <c r="C997" t="s">
+        <v>2406</v>
+      </c>
+      <c r="D997" t="s">
+        <v>2407</v>
+      </c>
+      <c r="E997" t="s">
+        <v>261</v>
+      </c>
+      <c r="F997" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/alerts-metric-create-templates</v>
+      </c>
+    </row>
+    <row r="998" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A998" s="1">
+        <v>43902.067569444444</v>
+      </c>
+      <c r="B998" t="s">
+        <v>12</v>
+      </c>
+      <c r="C998" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D998" t="s">
+        <v>2409</v>
+      </c>
+      <c r="E998" t="s">
+        <v>2356</v>
+      </c>
+      <c r="F998" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/export-telemetry</v>
+      </c>
+    </row>
+    <row r="999" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A999" s="1">
+        <v>43901.993761574071</v>
+      </c>
+      <c r="B999" t="s">
+        <v>54</v>
+      </c>
+      <c r="C999" t="s">
+        <v>2410</v>
+      </c>
+      <c r="D999" t="s">
+        <v>2411</v>
+      </c>
+      <c r="E999" t="s">
+        <v>42</v>
+      </c>
+      <c r="F999" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/metrics-supported</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1000" s="1">
+        <v>43901.707280092596</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>2413</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>2414</v>
+      </c>
+      <c r="F1000" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/vminsights-enable-overview</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1001" s="1">
+        <v>43901.616747685184</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>2415</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>2416</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1001" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/network-performance-monitor-faq</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1002" s="1">
+        <v>43901.504942129628</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>2417</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>2418</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1002" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/powershell-workspace-configuration</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1003" s="1">
+        <v>43901.461076388892</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>2419</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>2420</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1003" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/powershell-workspace-configuration</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1004" s="1">
+        <v>43901.327233796299</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>2421</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>2422</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>2423</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>2424</v>
+      </c>
+      <c r="F1004" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/docker</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1005" s="1">
+        <v>43900.933761574073</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>2425</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>2426</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1005" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/template-workspace-configuration</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1006" s="1">
+        <v>43900.898680555554</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>2427</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>2428</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>2362</v>
+      </c>
+      <c r="F1006" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/diagnostics-extension-schema-windows</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1007" s="1">
+        <v>43900.347662037035</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>2431</v>
+      </c>
+      <c r="F1007" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/azure-sql</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1008" s="1">
+        <v>43900.007569444446</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>2432</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>2433</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1008" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/change-analysis</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1009" s="1">
+        <v>43896.705439814818</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>2434</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>2435</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>2436</v>
+      </c>
+      <c r="F1009" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/alerts-enable-template</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1010" s="1">
+        <v>43896.228668981479</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>2437</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>2438</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>2356</v>
+      </c>
+      <c r="F1010" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/export-telemetry</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1011" s="1">
+        <v>43895.836273148147</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D1011" t="s">
+        <v>2440</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>398</v>
+      </c>
+      <c r="F1011" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/app-map</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1012" s="1">
+        <v>43895.752638888887</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>2441</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>2442</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1012" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/diagnostic-settings-template</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1013" s="1">
+        <v>43895.6796875</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>2443</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>2444</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>2445</v>
+      </c>
+      <c r="F1013" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/diagnostic-settings-legacy</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1014" s="1">
+        <v>43895.678865740738</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>2446</v>
+      </c>
+      <c r="D1014" t="s">
+        <v>2447</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>2448</v>
+      </c>
+      <c r="F1014" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/container-insights-overview</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1015" s="1">
+        <v>43895.517916666664</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>2450</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>2414</v>
+      </c>
+      <c r="F1015" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/vminsights-enable-overview</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1016" s="1">
+        <v>43894.846655092595</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>2451</v>
+      </c>
+      <c r="D1016" t="s">
+        <v>2452</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1016" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/diagnostic-settings</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1017" s="1">
+        <v>43894.663263888891</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>2453</v>
+      </c>
+      <c r="D1017" t="s">
+        <v>2454</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>2455</v>
+      </c>
+      <c r="F1017" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/automate-custom-reports</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1018" s="1">
+        <v>43894.244351851848</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>2456</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>2457</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1018" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/ip-addresses</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1019" s="1">
+        <v>43893.624374999999</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>2458</v>
+      </c>
+      <c r="D1019" t="s">
+        <v>2459</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>2460</v>
+      </c>
+      <c r="F1019" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/vminsights-health</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1020" s="1">
+        <v>43893.558854166666</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>2461</v>
+      </c>
+      <c r="D1020" t="s">
+        <v>2462</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>2340</v>
+      </c>
+      <c r="F1020" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/powerbi</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1021" s="1">
+        <v>43893.285034722219</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>2463</v>
+      </c>
+      <c r="D1021" t="s">
+        <v>2464</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>2465</v>
+      </c>
+      <c r="F1021" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/opencensus-go</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1022" s="1">
+        <v>43893.284074074072</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>2466</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>2467</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>2468</v>
+      </c>
+      <c r="F1022" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/app/opencensus-local-forwarder</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1023" s="1">
+        <v>43892.800798611112</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>2469</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>2470</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>2471</v>
+      </c>
+      <c r="F1023" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/resource-logs-collect-storage</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1024" s="1">
+        <v>43892.58084490741</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>2472</v>
+      </c>
+      <c r="D1024" t="s">
+        <v>2473</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>2474</v>
+      </c>
+      <c r="F1024" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/solutions-resources-searches-alerts</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1025" s="1">
+        <v>43892.41002314815</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>2475</v>
+      </c>
+      <c r="D1025" t="s">
+        <v>2476</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>2477</v>
+      </c>
+      <c r="F1025" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/insights/sql-assessment</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1026" s="1">
+        <v>43892.044166666667</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>2478</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>2479</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1026" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/platform/metrics-supported</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1027" s="1">
+        <v>43891.592048611114</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>2480</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>2481</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>2482</v>
+      </c>
+      <c r="F1027" t="str">
+        <f t="shared" si="16"/>
+        <v>http://docs.microsoft.com/azure/azure-monitor/azure-monitor/learn/tutorial-resource-logs</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1028" s="1"/>
     </row>
-    <row r="1029" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1029" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1029" s="1"/>
     </row>
-    <row r="1030" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1030" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1030" s="1"/>
     </row>
-    <row r="1031" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1031" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1031" s="1"/>
     </row>
-    <row r="1032" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1032" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1032" s="1"/>
     </row>
-    <row r="1033" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1033" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1033" s="1"/>
     </row>
-    <row r="1034" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1034" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1034" s="1"/>
     </row>
-    <row r="1035" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1035" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1035" s="1"/>
     </row>
-    <row r="1036" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1036" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1036" s="1"/>
     </row>
-    <row r="1037" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1037" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1037" s="1"/>
     </row>
-    <row r="1038" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1038" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1038" s="1"/>
     </row>
-    <row r="1039" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1039" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1039" s="1"/>
     </row>
-    <row r="1040" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1040" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1040" s="1"/>
     </row>
     <row r="1041" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>